<commit_message>
pas de deux named cells : datum, domare, firstvaulter
</commit_message>
<xml_diff>
--- a/mallar/Protokoll_2015_Pas_de_deux_klass_justerad 2017-05-30.xlsx
+++ b/mallar/Protokoll_2015_Pas_de_deux_klass_justerad 2017-05-30.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -21,6 +21,15 @@
     <definedName name="bord" localSheetId="3">'Pas-de-Deux art'!$L$3</definedName>
     <definedName name="bord" localSheetId="1">'Pas-de-Deux Häst'!$L$3</definedName>
     <definedName name="bord" localSheetId="2">'Pas-de-Deux tekn'!$L$3</definedName>
+    <definedName name="datum" localSheetId="3">'Pas-de-Deux art'!$C$4</definedName>
+    <definedName name="datum" localSheetId="1">'Pas-de-Deux Häst'!$C$4</definedName>
+    <definedName name="datum" localSheetId="2">'Pas-de-Deux tekn'!$C$4</definedName>
+    <definedName name="domare" localSheetId="3">'Pas-de-Deux art'!$C$27</definedName>
+    <definedName name="domare" localSheetId="1">'Pas-de-Deux Häst'!$C$30</definedName>
+    <definedName name="domare" localSheetId="2">'Pas-de-Deux tekn'!$C$36</definedName>
+    <definedName name="firstvaulter" localSheetId="3">'Pas-de-Deux art'!$J$7</definedName>
+    <definedName name="firstvaulter" localSheetId="1">'Pas-de-Deux Häst'!$J$7</definedName>
+    <definedName name="firstvaulter" localSheetId="2">'Pas-de-Deux tekn'!$J$7</definedName>
     <definedName name="id" localSheetId="3">'Pas-de-Deux art'!$U$1</definedName>
     <definedName name="id" localSheetId="1">'Pas-de-Deux Häst'!$U$1</definedName>
     <definedName name="id" localSheetId="2">'Pas-de-Deux tekn'!$U$1</definedName>
@@ -1810,15 +1819,102 @@
     <xf numFmtId="169" fontId="2" fillId="4" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    <xf numFmtId="169" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
@@ -1841,98 +1937,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="169" fontId="2" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2967,7 +2976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -3039,10 +3048,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="189"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="189"/>
-      <c r="F5" s="189"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
+      <c r="F5" s="157"/>
       <c r="H5" s="35"/>
       <c r="I5" s="36" t="s">
         <v>11</v>
@@ -3080,10 +3089,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="189"/>
-      <c r="D8" s="189"/>
-      <c r="E8" s="189"/>
-      <c r="F8" s="189"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="157"/>
+      <c r="F8" s="157"/>
       <c r="G8" s="1"/>
       <c r="H8" s="5" t="s">
         <v>15</v>
@@ -3098,32 +3107,32 @@
         <v>17</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="189"/>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
-      <c r="F9" s="189"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="157"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="157"/>
       <c r="G9" s="1"/>
       <c r="H9" s="34"/>
-      <c r="I9" s="155"/>
-      <c r="J9" s="156"/>
-      <c r="K9" s="156"/>
-      <c r="L9" s="156"/>
+      <c r="I9" s="168"/>
+      <c r="J9" s="169"/>
+      <c r="K9" s="169"/>
+      <c r="L9" s="169"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="189"/>
-      <c r="F10" s="189"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="157"/>
+      <c r="E10" s="157"/>
+      <c r="F10" s="157"/>
       <c r="G10" s="1"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="156"/>
-      <c r="K10" s="156"/>
-      <c r="L10" s="156"/>
+      <c r="I10" s="168"/>
+      <c r="J10" s="169"/>
+      <c r="K10" s="169"/>
+      <c r="L10" s="169"/>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
@@ -3147,215 +3156,215 @@
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
-      <c r="H12" s="195" t="s">
+      <c r="H12" s="175" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="196"/>
-      <c r="J12" s="192" t="s">
+      <c r="I12" s="176"/>
+      <c r="J12" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="193"/>
-      <c r="L12" s="194"/>
+      <c r="K12" s="173"/>
+      <c r="L12" s="174"/>
     </row>
     <row r="13" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="174" t="s">
+      <c r="A13" s="177" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="178" t="s">
+      <c r="B13" s="167" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="178" t="s">
+      <c r="C13" s="167" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="178"/>
-      <c r="E13" s="178"/>
-      <c r="F13" s="164" t="s">
+      <c r="D13" s="167"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="193" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="165"/>
+      <c r="G13" s="194"/>
       <c r="H13" s="41"/>
       <c r="I13" s="42"/>
-      <c r="J13" s="168" t="s">
+      <c r="J13" s="165" t="s">
         <v>6</v>
       </c>
       <c r="K13" s="170"/>
-      <c r="L13" s="163">
+      <c r="L13" s="192">
         <f>ROUND(K13*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="175"/>
-      <c r="B14" s="180"/>
-      <c r="C14" s="180" t="s">
+      <c r="A14" s="178"/>
+      <c r="B14" s="181"/>
+      <c r="C14" s="181" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="180"/>
-      <c r="E14" s="180"/>
-      <c r="F14" s="166" t="s">
+      <c r="D14" s="181"/>
+      <c r="E14" s="181"/>
+      <c r="F14" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="167"/>
+      <c r="G14" s="164"/>
       <c r="H14" s="43"/>
       <c r="I14" s="44"/>
-      <c r="J14" s="169"/>
+      <c r="J14" s="166"/>
       <c r="K14" s="171"/>
-      <c r="L14" s="161"/>
+      <c r="L14" s="190"/>
     </row>
     <row r="15" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="175"/>
-      <c r="B15" s="180"/>
-      <c r="C15" s="180" t="s">
+      <c r="A15" s="178"/>
+      <c r="B15" s="181"/>
+      <c r="C15" s="181" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="180"/>
-      <c r="E15" s="180"/>
-      <c r="F15" s="166" t="s">
+      <c r="D15" s="181"/>
+      <c r="E15" s="181"/>
+      <c r="F15" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="167"/>
+      <c r="G15" s="164"/>
       <c r="H15" s="45"/>
       <c r="I15" s="46"/>
-      <c r="J15" s="169"/>
+      <c r="J15" s="166"/>
       <c r="K15" s="171"/>
-      <c r="L15" s="161"/>
+      <c r="L15" s="190"/>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="175"/>
-      <c r="B16" s="181" t="s">
+      <c r="A16" s="178"/>
+      <c r="B16" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="180" t="s">
+      <c r="C16" s="181" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="180"/>
-      <c r="E16" s="180"/>
-      <c r="F16" s="166" t="s">
+      <c r="D16" s="181"/>
+      <c r="E16" s="181"/>
+      <c r="F16" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="167"/>
+      <c r="G16" s="164"/>
       <c r="H16" s="47"/>
       <c r="I16" s="48"/>
-      <c r="J16" s="169" t="s">
+      <c r="J16" s="166" t="s">
         <v>7</v>
       </c>
       <c r="K16" s="171"/>
-      <c r="L16" s="161">
+      <c r="L16" s="190">
         <f>ROUND(K16*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="175"/>
-      <c r="B17" s="182"/>
-      <c r="C17" s="180" t="s">
+      <c r="A17" s="178"/>
+      <c r="B17" s="183"/>
+      <c r="C17" s="181" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="180"/>
-      <c r="E17" s="180"/>
-      <c r="F17" s="166" t="s">
+      <c r="D17" s="181"/>
+      <c r="E17" s="181"/>
+      <c r="F17" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="167"/>
+      <c r="G17" s="164"/>
       <c r="H17" s="43"/>
       <c r="I17" s="44"/>
-      <c r="J17" s="169"/>
+      <c r="J17" s="166"/>
       <c r="K17" s="171"/>
-      <c r="L17" s="161"/>
+      <c r="L17" s="190"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="176"/>
-      <c r="B18" s="183"/>
-      <c r="C18" s="177" t="s">
+      <c r="A18" s="179"/>
+      <c r="B18" s="184"/>
+      <c r="C18" s="158" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="177"/>
-      <c r="E18" s="177"/>
-      <c r="F18" s="157" t="s">
+      <c r="D18" s="158"/>
+      <c r="E18" s="158"/>
+      <c r="F18" s="159" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="158"/>
+      <c r="G18" s="160"/>
       <c r="H18" s="49"/>
       <c r="I18" s="50"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="173"/>
-      <c r="L18" s="162"/>
+      <c r="J18" s="195"/>
+      <c r="K18" s="196"/>
+      <c r="L18" s="191"/>
     </row>
     <row r="19" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="174" t="s">
+      <c r="A19" s="177" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="184" t="s">
+      <c r="B19" s="185" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="178" t="s">
+      <c r="C19" s="167" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="178"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="190" t="s">
+      <c r="D19" s="167"/>
+      <c r="E19" s="167"/>
+      <c r="F19" s="161" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="191"/>
+      <c r="G19" s="162"/>
       <c r="H19" s="51"/>
       <c r="I19" s="52"/>
-      <c r="J19" s="168" t="s">
+      <c r="J19" s="165" t="s">
         <v>78</v>
       </c>
       <c r="K19" s="170"/>
-      <c r="L19" s="163">
+      <c r="L19" s="192">
         <f>ROUND(K19*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="175"/>
-      <c r="B20" s="185"/>
-      <c r="C20" s="180" t="s">
+      <c r="A20" s="178"/>
+      <c r="B20" s="186"/>
+      <c r="C20" s="181" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="180"/>
-      <c r="E20" s="180"/>
-      <c r="F20" s="166" t="s">
+      <c r="D20" s="181"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="163" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="167"/>
+      <c r="G20" s="164"/>
       <c r="H20" s="43"/>
       <c r="I20" s="44"/>
-      <c r="J20" s="169"/>
+      <c r="J20" s="166"/>
       <c r="K20" s="171"/>
-      <c r="L20" s="161"/>
+      <c r="L20" s="190"/>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="175"/>
-      <c r="B21" s="186"/>
-      <c r="C21" s="180" t="s">
+      <c r="A21" s="178"/>
+      <c r="B21" s="187"/>
+      <c r="C21" s="181" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="180"/>
-      <c r="E21" s="180"/>
-      <c r="F21" s="166" t="s">
+      <c r="D21" s="181"/>
+      <c r="E21" s="181"/>
+      <c r="F21" s="163" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="167"/>
+      <c r="G21" s="164"/>
       <c r="H21" s="45"/>
       <c r="I21" s="46"/>
-      <c r="J21" s="169"/>
+      <c r="J21" s="166"/>
       <c r="K21" s="171"/>
-      <c r="L21" s="161"/>
+      <c r="L21" s="190"/>
     </row>
     <row r="22" spans="1:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="176"/>
+      <c r="A22" s="179"/>
       <c r="B22" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="177"/>
-      <c r="D22" s="177"/>
-      <c r="E22" s="177"/>
-      <c r="F22" s="157" t="s">
+      <c r="C22" s="158"/>
+      <c r="D22" s="158"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="159" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="158"/>
+      <c r="G22" s="160"/>
       <c r="H22" s="54"/>
       <c r="I22" s="55"/>
       <c r="J22" s="56" t="s">
@@ -3374,15 +3383,15 @@
       <c r="B23" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="179" t="s">
+      <c r="C23" s="180" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="179"/>
-      <c r="E23" s="179"/>
-      <c r="F23" s="159" t="s">
+      <c r="D23" s="180"/>
+      <c r="E23" s="180"/>
+      <c r="F23" s="188" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="160"/>
+      <c r="G23" s="189"/>
       <c r="H23" s="58"/>
       <c r="I23" s="59"/>
       <c r="J23" s="60" t="s">
@@ -3421,11 +3430,11 @@
         <v>9</v>
       </c>
       <c r="J25" s="29"/>
-      <c r="K25" s="187">
+      <c r="K25" s="155">
         <f>SUM(L13:L23)</f>
         <v>0</v>
       </c>
-      <c r="L25" s="188"/>
+      <c r="L25" s="156"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E27" s="3"/>
@@ -3485,6 +3494,35 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="B13:B15"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
@@ -3501,35 +3539,6 @@
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="F17:G17"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3544,7 +3553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -3611,10 +3620,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="75"/>
-      <c r="C5" s="189"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="189"/>
-      <c r="F5" s="189"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
+      <c r="F5" s="157"/>
       <c r="H5" s="35"/>
       <c r="I5" s="36" t="s">
         <v>11</v>
@@ -3670,32 +3679,32 @@
         <v>17</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="189"/>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
-      <c r="F9" s="189"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="157"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="157"/>
       <c r="G9" s="1"/>
       <c r="H9" s="34"/>
-      <c r="I9" s="155"/>
-      <c r="J9" s="156"/>
-      <c r="K9" s="156"/>
-      <c r="L9" s="156"/>
+      <c r="I9" s="168"/>
+      <c r="J9" s="169"/>
+      <c r="K9" s="169"/>
+      <c r="L9" s="169"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="189"/>
-      <c r="F10" s="189"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="157"/>
+      <c r="E10" s="157"/>
+      <c r="F10" s="157"/>
       <c r="G10" s="1"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="156"/>
-      <c r="K10" s="156"/>
-      <c r="L10" s="156"/>
+      <c r="I10" s="168"/>
+      <c r="J10" s="169"/>
+      <c r="K10" s="169"/>
+      <c r="L10" s="169"/>
     </row>
     <row r="11" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="8"/>
@@ -4034,7 +4043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -4104,10 +4113,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="189"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="189"/>
-      <c r="F5" s="189"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
+      <c r="F5" s="157"/>
       <c r="H5" s="35"/>
       <c r="I5" s="36" t="s">
         <v>11</v>
@@ -4170,30 +4179,30 @@
         <v>17</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="189"/>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
-      <c r="F9" s="189"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="157"/>
+      <c r="E9" s="157"/>
+      <c r="F9" s="157"/>
       <c r="H9" s="31"/>
-      <c r="I9" s="155"/>
-      <c r="J9" s="156"/>
-      <c r="K9" s="156"/>
-      <c r="L9" s="156"/>
+      <c r="I9" s="168"/>
+      <c r="J9" s="169"/>
+      <c r="K9" s="169"/>
+      <c r="L9" s="169"/>
     </row>
     <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="189"/>
-      <c r="F10" s="189"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="157"/>
+      <c r="E10" s="157"/>
+      <c r="F10" s="157"/>
       <c r="H10" s="31"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="156"/>
-      <c r="K10" s="156"/>
-      <c r="L10" s="156"/>
+      <c r="I10" s="168"/>
+      <c r="J10" s="169"/>
+      <c r="K10" s="169"/>
+      <c r="L10" s="169"/>
     </row>
     <row r="11" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H11" s="8"/>
@@ -4376,12 +4385,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A16"/>
@@ -4389,6 +4392,12 @@
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B16:I16"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.98425196850393704" header="0.43307086614173229" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4400,6 +4409,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4465,25 +4492,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F9B768-A93D-4D4C-BBD7-D4CF83092D49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4498,27 +4530,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F9B768-A93D-4D4C-BBD7-D4CF83092D49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ändrat text av bedömning musik
</commit_message>
<xml_diff>
--- a/mallar/Protokoll_2015_Pas_de_deux_klass_justerad 2017-05-30.xlsx
+++ b/mallar/Protokoll_2015_Pas_de_deux_klass_justerad 2017-05-30.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlu\Documents\Source\Repos\voltigeScore\mallar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A3C17D-2F7B-4AB9-9233-5EEED6BFBA9D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-45" windowWidth="15195" windowHeight="4995" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-45" windowWidth="15195" windowHeight="4995" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="24" r:id="rId1"/>
@@ -39,13 +40,13 @@
     <definedName name="moment" localSheetId="3">'Pas-de-Deux art'!$L$5</definedName>
     <definedName name="moment" localSheetId="1">'Pas-de-Deux Häst'!$L$5</definedName>
     <definedName name="moment" localSheetId="2">'Pas-de-Deux tekn'!$L$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Pas-de-Deux art'!$A$1:$L$28</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Pas-de-Deux tekn'!$A$1:$L$47</definedName>
     <definedName name="result" localSheetId="3">'Pas-de-Deux art'!$L$21</definedName>
     <definedName name="result" localSheetId="1">'Pas-de-Deux Häst'!$K$25</definedName>
     <definedName name="result" localSheetId="2">'Pas-de-Deux tekn'!$L$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Pas-de-Deux art'!$A$1:$L$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Pas-de-Deux tekn'!$A$1:$L$47</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -340,32 +341,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Tolkning av musik</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-• Förmåga att förmedla musikens karaktär.
-• Uttrycksfullhet.
-• Rörelser och gester som kan kopplas till musiken.
-• Dräkter passar till temat av musiken.
-• Rörelser i harmoni med musiken.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>Kreatitivitet &amp; originalitet</t>
     </r>
     <r>
@@ -605,11 +580,36 @@
   <si>
     <t>Det finns även en tabell för domarrotation</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tolkning av musik</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+• Starkt engagemang till ett genomtänkt och utvecklat musikaliskt koncept
+• Fängslande tolkning av musiken
+• Stor variation av uttryck som speglar olika typer av musik samt förändringar i musiken
+• Komplext kroppsspråk samt gester och rörelser i många olika riktningar.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
@@ -1819,6 +1819,100 @@
     <xf numFmtId="169" fontId="2" fillId="4" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1828,46 +1922,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="2" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1883,66 +1943,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1984,12 +1984,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Dezimal 2" xfId="2"/>
-    <cellStyle name="Dezimal 2 2" xfId="5"/>
+    <cellStyle name="Dezimal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Dezimal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4"/>
-    <cellStyle name="Standard 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Standard 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Tusental" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2010,7 +2010,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2329,87 +2329,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="18" width="15.7109375" style="124" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="124"/>
+    <col min="1" max="18" width="15.73046875" style="124" customWidth="1"/>
+    <col min="19" max="16384" width="9.1328125" style="124"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="20.65" x14ac:dyDescent="0.6">
       <c r="A1" s="134" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="124" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="124" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="124" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="122" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="122" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A5" s="122" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="123" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="123"/>
+    </row>
+    <row r="9" spans="1:6" s="125" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="A9" s="125" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="123" t="s">
+    <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="126" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="123"/>
+    </row>
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="125" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="125" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="125" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="125"/>
+    </row>
+    <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="123" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="127" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="123"/>
-    </row>
-    <row r="9" spans="1:6" s="125" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="125" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="126" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="123"/>
-    </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="125" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="125" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="125" t="s">
-        <v>89</v>
-      </c>
-      <c r="E11" s="125"/>
-    </row>
-    <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="123" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="127" t="s">
+      <c r="C12" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="127" t="s">
+      <c r="D12" s="127" t="s">
         <v>96</v>
-      </c>
-      <c r="D12" s="127" t="s">
-        <v>97</v>
       </c>
       <c r="E12" s="130"/>
       <c r="F12" s="131"/>
     </row>
-    <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="123"/>
       <c r="B13" s="129"/>
       <c r="C13" s="129"/>
@@ -2417,135 +2417,135 @@
       <c r="E13" s="129"/>
       <c r="F13" s="131"/>
     </row>
-    <row r="15" spans="1:6" s="125" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="125" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A15" s="125" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="126" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="123"/>
       <c r="F16" s="126"/>
     </row>
-    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="125" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="125" t="s">
+      <c r="D17" s="125" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="125" t="s">
-        <v>89</v>
-      </c>
       <c r="E17" s="125" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F17" s="125"/>
       <c r="G17" s="125"/>
       <c r="H17" s="125"/>
       <c r="I17" s="125"/>
     </row>
-    <row r="18" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="123" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="127" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="127" t="s">
+      <c r="D18" s="127" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="127" t="s">
-        <v>97</v>
-      </c>
       <c r="E18" s="127" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" s="130"/>
       <c r="G18" s="129"/>
       <c r="H18" s="129"/>
       <c r="I18" s="129"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B19" s="129"/>
       <c r="C19" s="129"/>
       <c r="D19" s="129"/>
       <c r="E19" s="129"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B20" s="129"/>
       <c r="C20" s="129"/>
       <c r="D20" s="129"/>
       <c r="E20" s="129"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B21" s="129"/>
       <c r="C21" s="129"/>
       <c r="D21" s="129"/>
       <c r="E21" s="129"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A22" s="125" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="126" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="123"/>
       <c r="F24" s="126" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="125" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="125" t="s">
+      <c r="C25" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="125" t="s">
+      <c r="D25" s="125" t="s">
         <v>88</v>
-      </c>
-      <c r="D25" s="125" t="s">
-        <v>89</v>
       </c>
       <c r="E25" s="125"/>
       <c r="F25" s="125" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="125" t="s">
+      <c r="H25" s="125" t="s">
         <v>88</v>
       </c>
-      <c r="H25" s="125" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="123" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="127" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="127" t="s">
+      <c r="D26" s="127" t="s">
         <v>96</v>
-      </c>
-      <c r="D26" s="127" t="s">
-        <v>97</v>
       </c>
       <c r="E26" s="128"/>
       <c r="F26" s="127" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="127" t="s">
+      <c r="H26" s="127" t="s">
         <v>96</v>
       </c>
-      <c r="H26" s="127" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="123"/>
       <c r="B27" s="129"/>
       <c r="C27" s="129"/>
@@ -2555,415 +2555,415 @@
       <c r="G27" s="129"/>
       <c r="H27" s="129"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A29" s="125" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="126" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" s="123"/>
       <c r="F31" s="126" t="s">
+        <v>85</v>
+      </c>
+      <c r="J31" s="126"/>
+    </row>
+    <row r="32" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="125" t="s">
         <v>86</v>
       </c>
-      <c r="J31" s="126"/>
-    </row>
-    <row r="32" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="125" t="s">
+      <c r="C32" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="125" t="s">
+      <c r="D32" s="125" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="125" t="s">
-        <v>89</v>
-      </c>
       <c r="E32" s="125" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F32" s="125" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="G32" s="125" t="s">
+      <c r="H32" s="125" t="s">
         <v>88</v>
       </c>
-      <c r="H32" s="125" t="s">
-        <v>89</v>
-      </c>
       <c r="I32" s="125" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J32" s="125"/>
       <c r="K32" s="125"/>
       <c r="L32" s="125"/>
       <c r="M32" s="125"/>
     </row>
-    <row r="33" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="123" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" s="127" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="127" t="s">
+      <c r="D33" s="127" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="127" t="s">
-        <v>97</v>
-      </c>
       <c r="E33" s="127" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="127" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33" s="127" t="s">
+        <v>95</v>
+      </c>
+      <c r="H33" s="127" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="127" t="s">
+      <c r="I33" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="127" t="s">
-        <v>96</v>
-      </c>
-      <c r="H33" s="127" t="s">
-        <v>97</v>
-      </c>
-      <c r="I33" s="127" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="123" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:9" s="123" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A36" s="122" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="137" customFormat="1" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="137" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A37" s="136" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="136" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="136" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="136" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="136" t="s">
+        <v>90</v>
+      </c>
+      <c r="F37" s="136" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="136" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="136" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="136" t="s">
-        <v>89</v>
-      </c>
-      <c r="E37" s="136" t="s">
-        <v>91</v>
-      </c>
-      <c r="F37" s="136" t="s">
+    </row>
+    <row r="38" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="132" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="132" t="s">
+      <c r="B38" s="132" t="s">
         <v>102</v>
       </c>
-      <c r="B38" s="132" t="s">
+      <c r="C38" s="132" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="132" t="s">
+      <c r="D38" s="132" t="s">
         <v>104</v>
       </c>
-      <c r="D38" s="132" t="s">
+      <c r="E38" s="132" t="s">
         <v>105</v>
       </c>
-      <c r="E38" s="132" t="s">
+      <c r="F38" s="132" t="s">
         <v>106</v>
       </c>
-      <c r="F38" s="132" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:9" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="132"/>
       <c r="B39" s="132"/>
       <c r="C39" s="132"/>
       <c r="D39" s="132"/>
       <c r="E39" s="132"/>
       <c r="F39" s="133" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="122" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="122" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A42" s="122" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="125" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A43" s="138" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A44" s="140" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="141" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" s="125" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="138" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="140" t="s">
-        <v>123</v>
-      </c>
-      <c r="B44" s="141" t="s">
+      <c r="C44" s="141" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" s="141" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="141" t="s">
-        <v>106</v>
-      </c>
-      <c r="D44" s="141" t="s">
+      <c r="E44" s="141" t="s">
         <v>114</v>
       </c>
-      <c r="E44" s="141" t="s">
+    </row>
+    <row r="45" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="142" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="142" t="s">
+      <c r="B45" s="142" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="142" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" s="142" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="B45" s="142" t="s">
-        <v>119</v>
-      </c>
-      <c r="C45" s="142" t="s">
-        <v>118</v>
-      </c>
-      <c r="D45" s="142" t="s">
-        <v>120</v>
-      </c>
-      <c r="E45" s="142" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="143"/>
       <c r="B46" s="142" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C46" s="146" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" s="146" t="s">
         <v>126</v>
       </c>
-      <c r="D46" s="146" t="s">
-        <v>127</v>
-      </c>
       <c r="E46" s="142" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="144"/>
       <c r="B47" s="145"/>
       <c r="C47" s="145"/>
       <c r="D47" s="145"/>
       <c r="E47" s="145"/>
     </row>
-    <row r="48" spans="1:9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A48" s="140" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B48" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="141" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="141" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="141" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" s="141" t="s">
+      <c r="E48" s="141" t="s">
         <v>114</v>
       </c>
-      <c r="E48" s="141" t="s">
+    </row>
+    <row r="49" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="142" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="142" t="s">
+      <c r="B49" s="142" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="142" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="142" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="B49" s="142" t="s">
-        <v>119</v>
-      </c>
-      <c r="C49" s="142" t="s">
-        <v>118</v>
-      </c>
-      <c r="D49" s="142" t="s">
-        <v>120</v>
-      </c>
-      <c r="E49" s="142" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="143"/>
       <c r="B50" s="142" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C50" s="146" t="s">
+        <v>125</v>
+      </c>
+      <c r="D50" s="146" t="s">
         <v>126</v>
       </c>
-      <c r="D50" s="146" t="s">
-        <v>127</v>
-      </c>
       <c r="E50" s="142" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="142" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="142" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="142" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="142" t="s">
+        <v>118</v>
+      </c>
+      <c r="E51" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="B51" s="142" t="s">
-        <v>118</v>
-      </c>
-      <c r="C51" s="142" t="s">
-        <v>120</v>
-      </c>
-      <c r="D51" s="142" t="s">
-        <v>119</v>
-      </c>
-      <c r="E51" s="142" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="143"/>
       <c r="B52" s="142" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="146" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="146" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" s="142" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="139" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A55" s="138" t="s">
         <v>121</v>
       </c>
-      <c r="C52" s="146" t="s">
-        <v>126</v>
-      </c>
-      <c r="D52" s="146" t="s">
-        <v>127</v>
-      </c>
-      <c r="E52" s="142" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="139" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="138" t="s">
+    </row>
+    <row r="56" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.4">
+      <c r="A56" s="140" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="140" t="s">
-        <v>123</v>
-      </c>
       <c r="B56" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="141" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" s="141" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="141" t="s">
-        <v>106</v>
-      </c>
-      <c r="D56" s="141" t="s">
+      <c r="E56" s="141" t="s">
         <v>114</v>
       </c>
-      <c r="E56" s="141" t="s">
+    </row>
+    <row r="57" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="142" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="142" t="s">
+      <c r="B57" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="B57" s="142" t="s">
+      <c r="C57" s="142" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="142" t="s">
+      <c r="D57" s="142" t="s">
         <v>118</v>
       </c>
-      <c r="D57" s="142" t="s">
+      <c r="E57" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="E57" s="142" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="143"/>
       <c r="B58" s="142" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C58" s="146" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="146" t="s">
         <v>126</v>
       </c>
-      <c r="D58" s="146" t="s">
-        <v>127</v>
-      </c>
       <c r="E58" s="146" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.4">
       <c r="A60" s="140" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B60" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="C60" s="141" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60" s="141" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="141" t="s">
-        <v>106</v>
-      </c>
-      <c r="D60" s="141" t="s">
+      <c r="E60" s="141" t="s">
         <v>114</v>
       </c>
-      <c r="E60" s="141" t="s">
+    </row>
+    <row r="61" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="142" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="142" t="s">
+      <c r="B61" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="142" t="s">
+      <c r="C61" s="142" t="s">
         <v>117</v>
       </c>
-      <c r="C61" s="142" t="s">
+      <c r="D61" s="142" t="s">
         <v>118</v>
       </c>
-      <c r="D61" s="142" t="s">
+      <c r="E61" s="142" t="s">
         <v>119</v>
       </c>
-      <c r="E61" s="142" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="143"/>
       <c r="B62" s="142" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C62" s="146" t="s">
+        <v>125</v>
+      </c>
+      <c r="D62" s="146" t="s">
         <v>126</v>
       </c>
-      <c r="D62" s="146" t="s">
-        <v>127</v>
-      </c>
       <c r="E62" s="146" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="142" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" s="142" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="142" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="142" t="s">
+        <v>117</v>
+      </c>
+      <c r="E63" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="B63" s="142" t="s">
-        <v>120</v>
-      </c>
-      <c r="C63" s="142" t="s">
-        <v>119</v>
-      </c>
-      <c r="D63" s="142" t="s">
-        <v>118</v>
-      </c>
-      <c r="E63" s="142" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="143"/>
       <c r="B64" s="142" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C64" s="146" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" s="146" t="s">
         <v>126</v>
       </c>
-      <c r="D64" s="146" t="s">
-        <v>127</v>
-      </c>
       <c r="E64" s="146" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2973,33 +2973,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.59765625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="10.73046875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="5.73046875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.59765625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.73046875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>51</v>
       </c>
@@ -3007,26 +3007,26 @@
       <c r="C2" s="3"/>
       <c r="H2" s="35"/>
       <c r="I2" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2" s="37"/>
       <c r="K2" s="38"/>
       <c r="L2" s="38"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="35"/>
       <c r="I3" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" s="37"/>
       <c r="K3" s="38"/>
       <c r="L3" s="38"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -3043,15 +3043,15 @@
       <c r="K4" s="38"/>
       <c r="L4" s="38"/>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
+      <c r="C5" s="189"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="189"/>
+      <c r="F5" s="189"/>
       <c r="H5" s="35"/>
       <c r="I5" s="36" t="s">
         <v>11</v>
@@ -3060,13 +3060,13 @@
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -3084,15 +3084,15 @@
       <c r="K7" s="64"/>
       <c r="L7" s="64"/>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="157"/>
-      <c r="D8" s="157"/>
-      <c r="E8" s="157"/>
-      <c r="F8" s="157"/>
+      <c r="C8" s="189"/>
+      <c r="D8" s="189"/>
+      <c r="E8" s="189"/>
+      <c r="F8" s="189"/>
       <c r="G8" s="1"/>
       <c r="H8" s="5" t="s">
         <v>15</v>
@@ -3102,39 +3102,39 @@
       <c r="K8" s="63"/>
       <c r="L8" s="63"/>
     </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
+      <c r="C9" s="189"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="189"/>
       <c r="G9" s="1"/>
       <c r="H9" s="34"/>
-      <c r="I9" s="168"/>
-      <c r="J9" s="169"/>
-      <c r="K9" s="169"/>
-      <c r="L9" s="169"/>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="155"/>
+      <c r="J9" s="156"/>
+      <c r="K9" s="156"/>
+      <c r="L9" s="156"/>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="157"/>
-      <c r="D10" s="157"/>
-      <c r="E10" s="157"/>
-      <c r="F10" s="157"/>
+      <c r="C10" s="189"/>
+      <c r="D10" s="189"/>
+      <c r="E10" s="189"/>
+      <c r="F10" s="189"/>
       <c r="G10" s="1"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="168"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="169"/>
-      <c r="L10" s="169"/>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="155"/>
+      <c r="J10" s="156"/>
+      <c r="K10" s="156"/>
+      <c r="L10" s="156"/>
+    </row>
+    <row r="11" spans="1:13" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="112"/>
@@ -3148,7 +3148,7 @@
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="40"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
@@ -3156,215 +3156,215 @@
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
-      <c r="H12" s="175" t="s">
+      <c r="H12" s="195" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="176"/>
-      <c r="J12" s="172" t="s">
+      <c r="I12" s="196"/>
+      <c r="J12" s="192" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="173"/>
-      <c r="L12" s="174"/>
-    </row>
-    <row r="13" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="177" t="s">
+      <c r="K12" s="193"/>
+      <c r="L12" s="194"/>
+    </row>
+    <row r="13" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="174" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="167" t="s">
+      <c r="B13" s="178" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="167" t="s">
+      <c r="C13" s="178" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="167"/>
-      <c r="E13" s="167"/>
-      <c r="F13" s="193" t="s">
+      <c r="D13" s="178"/>
+      <c r="E13" s="178"/>
+      <c r="F13" s="164" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="194"/>
+      <c r="G13" s="165"/>
       <c r="H13" s="41"/>
       <c r="I13" s="42"/>
-      <c r="J13" s="165" t="s">
+      <c r="J13" s="168" t="s">
         <v>6</v>
       </c>
       <c r="K13" s="170"/>
-      <c r="L13" s="192">
+      <c r="L13" s="163">
         <f>ROUND(K13*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="178"/>
-      <c r="B14" s="181"/>
-      <c r="C14" s="181" t="s">
+    <row r="14" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="175"/>
+      <c r="B14" s="180"/>
+      <c r="C14" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="181"/>
-      <c r="E14" s="181"/>
-      <c r="F14" s="163" t="s">
+      <c r="D14" s="180"/>
+      <c r="E14" s="180"/>
+      <c r="F14" s="166" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="164"/>
+      <c r="G14" s="167"/>
       <c r="H14" s="43"/>
       <c r="I14" s="44"/>
-      <c r="J14" s="166"/>
+      <c r="J14" s="169"/>
       <c r="K14" s="171"/>
-      <c r="L14" s="190"/>
-    </row>
-    <row r="15" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="178"/>
-      <c r="B15" s="181"/>
-      <c r="C15" s="181" t="s">
+      <c r="L14" s="161"/>
+    </row>
+    <row r="15" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="175"/>
+      <c r="B15" s="180"/>
+      <c r="C15" s="180" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="181"/>
-      <c r="E15" s="181"/>
-      <c r="F15" s="163" t="s">
+      <c r="D15" s="180"/>
+      <c r="E15" s="180"/>
+      <c r="F15" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="164"/>
+      <c r="G15" s="167"/>
       <c r="H15" s="45"/>
       <c r="I15" s="46"/>
-      <c r="J15" s="166"/>
+      <c r="J15" s="169"/>
       <c r="K15" s="171"/>
-      <c r="L15" s="190"/>
-    </row>
-    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="178"/>
-      <c r="B16" s="182" t="s">
+      <c r="L15" s="161"/>
+    </row>
+    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="175"/>
+      <c r="B16" s="181" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="181" t="s">
+      <c r="C16" s="180" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="181"/>
-      <c r="E16" s="181"/>
-      <c r="F16" s="163" t="s">
+      <c r="D16" s="180"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="166" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="164"/>
+      <c r="G16" s="167"/>
       <c r="H16" s="47"/>
       <c r="I16" s="48"/>
-      <c r="J16" s="166" t="s">
+      <c r="J16" s="169" t="s">
         <v>7</v>
       </c>
       <c r="K16" s="171"/>
-      <c r="L16" s="190">
+      <c r="L16" s="161">
         <f>ROUND(K16*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="178"/>
-      <c r="B17" s="183"/>
-      <c r="C17" s="181" t="s">
+    <row r="17" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="175"/>
+      <c r="B17" s="182"/>
+      <c r="C17" s="180" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="181"/>
-      <c r="E17" s="181"/>
-      <c r="F17" s="163" t="s">
+      <c r="D17" s="180"/>
+      <c r="E17" s="180"/>
+      <c r="F17" s="166" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="164"/>
+      <c r="G17" s="167"/>
       <c r="H17" s="43"/>
       <c r="I17" s="44"/>
-      <c r="J17" s="166"/>
+      <c r="J17" s="169"/>
       <c r="K17" s="171"/>
-      <c r="L17" s="190"/>
-    </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="179"/>
-      <c r="B18" s="184"/>
-      <c r="C18" s="158" t="s">
+      <c r="L17" s="161"/>
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="176"/>
+      <c r="B18" s="183"/>
+      <c r="C18" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="158"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="159" t="s">
+      <c r="D18" s="177"/>
+      <c r="E18" s="177"/>
+      <c r="F18" s="157" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="160"/>
+      <c r="G18" s="158"/>
       <c r="H18" s="49"/>
       <c r="I18" s="50"/>
-      <c r="J18" s="195"/>
-      <c r="K18" s="196"/>
-      <c r="L18" s="191"/>
-    </row>
-    <row r="19" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="177" t="s">
+      <c r="J18" s="172"/>
+      <c r="K18" s="173"/>
+      <c r="L18" s="162"/>
+    </row>
+    <row r="19" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="174" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="185" t="s">
+      <c r="B19" s="184" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="167" t="s">
+      <c r="C19" s="178" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="167"/>
-      <c r="E19" s="167"/>
-      <c r="F19" s="161" t="s">
+      <c r="D19" s="178"/>
+      <c r="E19" s="178"/>
+      <c r="F19" s="190" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="162"/>
+      <c r="G19" s="191"/>
       <c r="H19" s="51"/>
       <c r="I19" s="52"/>
-      <c r="J19" s="165" t="s">
-        <v>78</v>
+      <c r="J19" s="168" t="s">
+        <v>77</v>
       </c>
       <c r="K19" s="170"/>
-      <c r="L19" s="192">
+      <c r="L19" s="163">
         <f>ROUND(K19*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="178"/>
-      <c r="B20" s="186"/>
-      <c r="C20" s="181" t="s">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="175"/>
+      <c r="B20" s="185"/>
+      <c r="C20" s="180" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="181"/>
-      <c r="E20" s="181"/>
-      <c r="F20" s="163" t="s">
+      <c r="D20" s="180"/>
+      <c r="E20" s="180"/>
+      <c r="F20" s="166" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="164"/>
+      <c r="G20" s="167"/>
       <c r="H20" s="43"/>
       <c r="I20" s="44"/>
-      <c r="J20" s="166"/>
+      <c r="J20" s="169"/>
       <c r="K20" s="171"/>
-      <c r="L20" s="190"/>
-    </row>
-    <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="178"/>
-      <c r="B21" s="187"/>
-      <c r="C21" s="181" t="s">
+      <c r="L20" s="161"/>
+    </row>
+    <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="175"/>
+      <c r="B21" s="186"/>
+      <c r="C21" s="180" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="181"/>
-      <c r="E21" s="181"/>
-      <c r="F21" s="163" t="s">
+      <c r="D21" s="180"/>
+      <c r="E21" s="180"/>
+      <c r="F21" s="166" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="164"/>
+      <c r="G21" s="167"/>
       <c r="H21" s="45"/>
       <c r="I21" s="46"/>
-      <c r="J21" s="166"/>
+      <c r="J21" s="169"/>
       <c r="K21" s="171"/>
-      <c r="L21" s="190"/>
-    </row>
-    <row r="22" spans="1:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="179"/>
+      <c r="L21" s="161"/>
+    </row>
+    <row r="22" spans="1:12" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="176"/>
       <c r="B22" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="158"/>
-      <c r="D22" s="158"/>
-      <c r="E22" s="158"/>
-      <c r="F22" s="159" t="s">
+      <c r="C22" s="177"/>
+      <c r="D22" s="177"/>
+      <c r="E22" s="177"/>
+      <c r="F22" s="157" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="160"/>
+      <c r="G22" s="158"/>
       <c r="H22" s="54"/>
       <c r="I22" s="55"/>
       <c r="J22" s="56" t="s">
@@ -3376,26 +3376,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="57" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="115" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="180" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="180"/>
-      <c r="E23" s="180"/>
-      <c r="F23" s="188" t="s">
+      <c r="D23" s="179"/>
+      <c r="E23" s="179"/>
+      <c r="F23" s="159" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="189"/>
+      <c r="G23" s="160"/>
       <c r="H23" s="58"/>
       <c r="I23" s="59"/>
       <c r="J23" s="60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K23" s="154"/>
       <c r="L23" s="61">
@@ -3403,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -3417,7 +3417,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -3430,13 +3430,13 @@
         <v>9</v>
       </c>
       <c r="J25" s="29"/>
-      <c r="K25" s="155">
+      <c r="K25" s="187">
         <f>SUM(L13:L23)</f>
         <v>0</v>
       </c>
-      <c r="L25" s="156"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="188"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -3446,7 +3446,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -3460,7 +3460,7 @@
       <c r="K28" s="65"/>
       <c r="L28" s="65"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -3474,7 +3474,7 @@
       <c r="K29" s="65"/>
       <c r="L29" s="65"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A30" s="30" t="s">
         <v>48</v>
       </c>
@@ -3494,35 +3494,6 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="L19:L21"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="B13:B15"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
@@ -3539,6 +3510,35 @@
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="L19:L21"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="F17:G17"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3550,55 +3550,55 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="3" customWidth="1"/>
-    <col min="5" max="7" width="7.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="3"/>
+    <col min="3" max="3" width="12.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="3" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="3" customWidth="1"/>
     <col min="8" max="8" width="7" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="9" width="7.265625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="4.73046875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.265625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.73046875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="74" t="s">
         <v>51</v>
       </c>
       <c r="H2" s="35"/>
       <c r="I2" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2" s="37"/>
       <c r="K2" s="38"/>
       <c r="L2" s="38"/>
     </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>52</v>
       </c>
       <c r="H3" s="35"/>
       <c r="I3" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" s="37"/>
       <c r="K3" s="38"/>
       <c r="L3" s="38"/>
     </row>
-    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -3615,15 +3615,15 @@
       <c r="K4" s="38"/>
       <c r="L4" s="38"/>
     </row>
-    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="75" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="75"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
+      <c r="C5" s="189"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="189"/>
+      <c r="F5" s="189"/>
       <c r="H5" s="35"/>
       <c r="I5" s="36" t="s">
         <v>11</v>
@@ -3632,11 +3632,11 @@
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H6" s="121"/>
       <c r="I6" s="121"/>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -3655,7 +3655,7 @@
       <c r="L7" s="64"/>
       <c r="M7" s="112"/>
     </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -3674,46 +3674,46 @@
       <c r="L8" s="63"/>
       <c r="M8" s="112"/>
     </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
+      <c r="C9" s="189"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="189"/>
       <c r="G9" s="1"/>
       <c r="H9" s="34"/>
-      <c r="I9" s="168"/>
-      <c r="J9" s="169"/>
-      <c r="K9" s="169"/>
-      <c r="L9" s="169"/>
-    </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="155"/>
+      <c r="J9" s="156"/>
+      <c r="K9" s="156"/>
+      <c r="L9" s="156"/>
+    </row>
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="157"/>
-      <c r="D10" s="157"/>
-      <c r="E10" s="157"/>
-      <c r="F10" s="157"/>
+      <c r="C10" s="189"/>
+      <c r="D10" s="189"/>
+      <c r="E10" s="189"/>
+      <c r="F10" s="189"/>
       <c r="G10" s="1"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="168"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="169"/>
-      <c r="L10" s="169"/>
-    </row>
-    <row r="11" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="155"/>
+      <c r="J10" s="156"/>
+      <c r="K10" s="156"/>
+      <c r="L10" s="156"/>
+    </row>
+    <row r="11" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
         <v>53</v>
       </c>
@@ -3729,7 +3729,7 @@
       <c r="K12" s="79"/>
       <c r="L12" s="80"/>
     </row>
-    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="67"/>
       <c r="B13" s="68"/>
       <c r="C13" s="68"/>
@@ -3743,7 +3743,7 @@
       <c r="K13" s="70"/>
       <c r="L13" s="81"/>
     </row>
-    <row r="14" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="67"/>
       <c r="B14" s="68"/>
       <c r="C14" s="68"/>
@@ -3757,7 +3757,7 @@
       <c r="K14" s="68"/>
       <c r="L14" s="69"/>
     </row>
-    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="116" t="s">
         <v>50</v>
       </c>
@@ -3773,7 +3773,7 @@
       <c r="K15" s="119"/>
       <c r="L15" s="120"/>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="82" t="s">
         <v>54</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="L16" s="68"/>
       <c r="M16" s="68"/>
     </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="68"/>
       <c r="B17" s="68"/>
       <c r="C17" s="68"/>
@@ -3798,7 +3798,7 @@
       <c r="F17" s="68"/>
       <c r="G17" s="69"/>
       <c r="H17" s="103" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I17" s="83"/>
       <c r="K17" s="104" t="s">
@@ -3806,7 +3806,7 @@
       </c>
       <c r="M17" s="68"/>
     </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="105" t="s">
         <v>60</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="105" t="s">
         <v>61</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="105" t="s">
         <v>62</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="88" t="s">
         <v>65</v>
       </c>
@@ -3879,7 +3879,7 @@
       <c r="J21" s="109"/>
       <c r="K21" s="109"/>
     </row>
-    <row r="22" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G22" s="96" t="s">
         <v>64</v>
       </c>
@@ -3894,17 +3894,17 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" s="85" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="68"/>
       <c r="C25" s="68"/>
       <c r="D25" s="68"/>
@@ -3916,7 +3916,7 @@
       <c r="J25" s="86"/>
       <c r="K25" s="87"/>
     </row>
-    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="88" t="s">
         <v>57</v>
       </c>
@@ -3924,7 +3924,7 @@
       <c r="D26" s="90"/>
       <c r="E26" s="149"/>
       <c r="F26" s="88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G26" s="90"/>
       <c r="H26" s="91">
@@ -3941,7 +3941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B27" s="111"/>
       <c r="C27" s="111"/>
       <c r="D27" s="111"/>
@@ -3953,11 +3953,11 @@
       <c r="J27" s="93"/>
       <c r="K27" s="111"/>
     </row>
-    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="111"/>
       <c r="C28" s="111"/>
       <c r="D28" s="88" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E28" s="75"/>
       <c r="F28" s="75"/>
@@ -3967,7 +3967,7 @@
       <c r="J28" s="95"/>
       <c r="K28" s="72"/>
     </row>
-    <row r="29" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="68"/>
       <c r="C29" s="68"/>
       <c r="D29" s="68"/>
@@ -3978,7 +3978,7 @@
       <c r="I29" s="68"/>
       <c r="L29" s="84"/>
     </row>
-    <row r="30" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G30" s="96" t="s">
         <v>58</v>
       </c>
@@ -3993,8 +3993,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I32" s="100" t="s">
         <v>59</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>48</v>
       </c>
@@ -4040,31 +4040,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView showZeros="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="7.265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.73046875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.73046875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>51</v>
       </c>
@@ -4072,26 +4072,26 @@
       <c r="C2" s="3"/>
       <c r="H2" s="35"/>
       <c r="I2" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2" s="37"/>
       <c r="K2" s="38"/>
       <c r="L2" s="38"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>66</v>
       </c>
       <c r="H3" s="35"/>
       <c r="I3" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J3" s="37"/>
       <c r="K3" s="38"/>
       <c r="L3" s="38"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -4108,15 +4108,15 @@
       <c r="K4" s="38"/>
       <c r="L4" s="38"/>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
+      <c r="C5" s="189"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="189"/>
+      <c r="F5" s="189"/>
       <c r="H5" s="35"/>
       <c r="I5" s="36" t="s">
         <v>11</v>
@@ -4125,7 +4125,7 @@
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="76"/>
@@ -4138,7 +4138,7 @@
       <c r="K6" s="113"/>
       <c r="L6" s="113"/>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -4156,7 +4156,7 @@
       <c r="L7" s="64"/>
       <c r="M7" s="112"/>
     </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -4174,37 +4174,37 @@
       <c r="L8" s="63"/>
       <c r="M8" s="112"/>
     </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="157"/>
+      <c r="C9" s="189"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="189"/>
       <c r="H9" s="31"/>
-      <c r="I9" s="168"/>
-      <c r="J9" s="169"/>
-      <c r="K9" s="169"/>
-      <c r="L9" s="169"/>
-    </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="155"/>
+      <c r="J9" s="156"/>
+      <c r="K9" s="156"/>
+      <c r="L9" s="156"/>
+    </row>
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="157"/>
-      <c r="D10" s="157"/>
-      <c r="E10" s="157"/>
-      <c r="F10" s="157"/>
+      <c r="C10" s="189"/>
+      <c r="D10" s="189"/>
+      <c r="E10" s="189"/>
+      <c r="F10" s="189"/>
       <c r="H10" s="31"/>
-      <c r="I10" s="168"/>
-      <c r="J10" s="169"/>
-      <c r="K10" s="169"/>
-      <c r="L10" s="169"/>
-    </row>
-    <row r="11" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="155"/>
+      <c r="J10" s="156"/>
+      <c r="K10" s="156"/>
+      <c r="L10" s="156"/>
+    </row>
+    <row r="11" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -4213,12 +4213,12 @@
       </c>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="200" t="s">
         <v>67</v>
       </c>
       <c r="B12" s="203" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="204"/>
       <c r="D12" s="204"/>
@@ -4237,10 +4237,10 @@
       </c>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="201"/>
       <c r="B13" s="205" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="206"/>
       <c r="D13" s="206"/>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="200" t="s">
         <v>69</v>
       </c>
@@ -4283,10 +4283,10 @@
       </c>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="202"/>
       <c r="B15" s="198" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="C15" s="199"/>
       <c r="D15" s="199"/>
@@ -4305,10 +4305,10 @@
       </c>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="1:13" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="201"/>
       <c r="B16" s="209" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="206"/>
       <c r="D16" s="206"/>
@@ -4327,16 +4327,16 @@
       </c>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L17" s="26">
         <f>SUM(L12:L16)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L18" s="27"/>
     </row>
-    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="32" t="s">
         <v>56</v>
       </c>
@@ -4351,12 +4351,12 @@
       <c r="K19" s="13"/>
       <c r="L19" s="150"/>
     </row>
-    <row r="20" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L20" s="27"/>
     </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I21" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
@@ -4365,7 +4365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>48</v>
       </c>
@@ -4385,6 +4385,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A16"/>
@@ -4392,12 +4398,6 @@
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B16:I16"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.98425196850393704" header="0.43307086614173229" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4409,24 +4409,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4492,30 +4474,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F9B768-A93D-4D4C-BBD7-D4CF83092D49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4530,4 +4507,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F9B768-A93D-4D4C-BBD7-D4CF83092D49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>